<commit_message>
Started Working On Exporting SF4
</commit_message>
<xml_diff>
--- a/Project Files/Forms System Final/exports/jh_sf3.xlsx
+++ b/Project Files/Forms System Final/exports/jh_sf3.xlsx
@@ -108,16 +108,16 @@
     <t xml:space="preserve">FUMINO ONA FURAHASHI </t>
   </si>
   <si>
-    <t>ENG32</t>
-  </si>
-  <si>
-    <t>MATH31</t>
-  </si>
-  <si>
-    <t>FILIPINO-69</t>
-  </si>
-  <si>
-    <t>AP20</t>
+    <t>1. ENG32</t>
+  </si>
+  <si>
+    <t>2. MATH31</t>
+  </si>
+  <si>
+    <t>3. FILIPINO-69</t>
+  </si>
+  <si>
+    <t>4. AP20</t>
   </si>
   <si>
     <t>1</t>

</xml_diff>